<commit_message>
feat: finished cart and tests
</commit_message>
<xml_diff>
--- a/src/L5zero/messages.xlsx
+++ b/src/L5zero/messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rumyantsev\IdeaProjects\bookshop\src\L5zero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37278ABD-9B1C-4BC4-B011-B192279D88B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E641B1-5A4E-4BAE-87BA-D0FDB7BDD110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7710" yWindow="3720" windowWidth="17370" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6195" yWindow="3105" windowWidth="17370" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>key</t>
   </si>
@@ -226,6 +226,33 @@
   </si>
   <si>
     <t>Заказ не найден</t>
+  </si>
+  <si>
+    <t>cart_not_found</t>
+  </si>
+  <si>
+    <t>cart not found</t>
+  </si>
+  <si>
+    <t>Корзина не найдена</t>
+  </si>
+  <si>
+    <t>cart_item_not_found</t>
+  </si>
+  <si>
+    <t>cart item not found</t>
+  </si>
+  <si>
+    <t>Элемент корзины не найден</t>
+  </si>
+  <si>
+    <t>cart_item_already_exists</t>
+  </si>
+  <si>
+    <t>Item is already in your cart</t>
+  </si>
+  <si>
+    <t>Данный товар уже в корзине</t>
   </si>
 </sst>
 </file>
@@ -592,13 +619,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,6 +880,39 @@
         <v>66</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add e-mail account activation
</commit_message>
<xml_diff>
--- a/src/L5zero/messages.xlsx
+++ b/src/L5zero/messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rumyantsev\IdeaProjects\bookshop\src\L5zero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E641B1-5A4E-4BAE-87BA-D0FDB7BDD110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81164B7-CD56-436E-ABE2-898D7A583013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="3105" windowWidth="17370" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8025" yWindow="3540" windowWidth="17370" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,6 @@
     <t>ru</t>
   </si>
   <si>
-    <t>user registered successfully</t>
-  </si>
-  <si>
-    <t>Пользователь успешно зарегистрирован</t>
-  </si>
-  <si>
     <t>user_exists</t>
   </si>
   <si>
@@ -253,6 +247,12 @@
   </si>
   <si>
     <t>Данный товар уже в корзине</t>
+  </si>
+  <si>
+    <t>User registered successfully. Check your e-mail to complete registration.</t>
+  </si>
+  <si>
+    <t>Пользователь успешно зарегистрирован. Письмо с подтверждением регистрации от правлено вам на почту.</t>
   </si>
 </sst>
 </file>
@@ -622,10 +622,10 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,268 +649,268 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>